<commit_message>
changes of key figures
</commit_message>
<xml_diff>
--- a/key_figures1.xlsx
+++ b/key_figures1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\UNI\Master_Digital_Humanities\S1_WS2023\UE_Motion_Capture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F59AC-E687-468B-9D2B-D714E032CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67BAD4F-D7AF-4CA7-BAFC-CA6EA85722EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{F55C0E63-8286-4C99-8805-A4CBFE20548D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="14190" windowHeight="20970" xr2:uid="{F55C0E63-8286-4C99-8805-A4CBFE20548D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <t>music clip</t>
   </si>
   <si>
-    <t>after3</t>
+    <t>after 3 seconds</t>
   </si>
 </sst>
 </file>
@@ -7560,15 +7560,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>138966</xdr:colOff>
+      <xdr:colOff>1067043</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>48846</xdr:rowOff>
+      <xdr:rowOff>117231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238612</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>404689</xdr:colOff>
       <xdr:row>100</xdr:row>
-      <xdr:rowOff>28332</xdr:rowOff>
+      <xdr:rowOff>96717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7596,15 +7596,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>273538</xdr:colOff>
+      <xdr:colOff>884115</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>87923</xdr:rowOff>
+      <xdr:rowOff>170962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>373184</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>221761</xdr:colOff>
       <xdr:row>118</xdr:row>
-      <xdr:rowOff>67409</xdr:rowOff>
+      <xdr:rowOff>150448</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7953,12 +7953,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DE26DF-7610-41D0-B1E1-A0000CFD1B1E}">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100:D100"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
     <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>

</xml_diff>